<commit_message>
Updated timeframe in input files
</commit_message>
<xml_diff>
--- a/01_Input/Local_Counts/004_Merged.xlsx
+++ b/01_Input/Local_Counts/004_Merged.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\OneDrive - mail.uni-mannheim.de\Uni\Master\Semester 3\Teamproject\Towards-Sustainable-Cities-through-Simulation\01_Input\Local_Counts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailunimannheimde-my.sharepoint.com/personal/pstapf_mail_uni-mannheim_de/Documents/Uni/Master/Semester 3/Teamproject/Towards-Sustainable-Cities-through-Simulation/01_Input/Local_Counts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7826FCD7-9365-4955-90F4-51E39AF2F279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{7826FCD7-9365-4955-90F4-51E39AF2F279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9C570C9-5F56-4FDB-85AB-F51FB2CD2F9D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -147,12 +147,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </top>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
@@ -165,7 +165,7 @@
         <color theme="4" tint="0.39997558519241921"/>
       </right>
       <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
@@ -178,23 +178,34 @@
         <color theme="4" tint="0.39997558519241921"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
       <top style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
       </bottom>
       <diagonal/>
     </border>
@@ -202,24 +213,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +515,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection sqref="A1:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,45 +524,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>45271.305555555555</v>
-      </c>
-      <c r="B2" s="14">
-        <v>2</v>
-      </c>
-      <c r="C2" s="14">
+        <v>45271.3125</v>
+      </c>
+      <c r="B2" s="11">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11">
         <v>63</v>
       </c>
-      <c r="D2" s="14">
-        <v>0</v>
-      </c>
-      <c r="E2" s="14">
+      <c r="D2" s="11">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
         <v>27</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="11">
         <v>0</v>
       </c>
       <c r="G2" s="3">
@@ -561,21 +573,21 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>45271.3125</v>
-      </c>
-      <c r="B3" s="14">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14">
+        <v>45271.319444502318</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
         <v>96</v>
       </c>
-      <c r="D3" s="14">
-        <v>1</v>
-      </c>
-      <c r="E3" s="14">
+      <c r="D3" s="11">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11">
         <v>24</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="11">
         <v>0</v>
       </c>
       <c r="G3" s="3">
@@ -586,21 +598,21 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>45271.319444502318</v>
-      </c>
-      <c r="B4" s="14">
-        <v>0</v>
-      </c>
-      <c r="C4" s="14">
+        <v>45271.326389004629</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11">
         <v>88</v>
       </c>
-      <c r="D4" s="14">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14">
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
         <v>29</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="11">
         <v>1</v>
       </c>
       <c r="G4" s="3">
@@ -611,21 +623,21 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>45271.326389004629</v>
-      </c>
-      <c r="B5" s="14">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14">
+        <v>45271.333333506947</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11">
         <v>83</v>
       </c>
-      <c r="D5" s="14">
-        <v>1</v>
-      </c>
-      <c r="E5" s="14">
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
         <v>28</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="11">
         <v>1</v>
       </c>
       <c r="G5" s="3">
@@ -636,21 +648,21 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>45271.333333506947</v>
-      </c>
-      <c r="B6" s="14">
-        <v>1</v>
-      </c>
-      <c r="C6" s="14">
+        <v>45271.340278009258</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
         <v>78</v>
       </c>
-      <c r="D6" s="14">
-        <v>1</v>
-      </c>
-      <c r="E6" s="14">
+      <c r="D6" s="11">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11">
         <v>37</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="11">
         <v>2</v>
       </c>
       <c r="G6" s="3">
@@ -661,21 +673,21 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>45271.340278009258</v>
-      </c>
-      <c r="B7" s="14">
-        <v>0</v>
-      </c>
-      <c r="C7" s="14">
+        <v>45271.347222511577</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11">
         <v>76</v>
       </c>
-      <c r="D7" s="14">
-        <v>2</v>
-      </c>
-      <c r="E7" s="14">
+      <c r="D7" s="11">
+        <v>2</v>
+      </c>
+      <c r="E7" s="11">
         <v>27</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="11">
         <v>2</v>
       </c>
       <c r="G7" s="3">
@@ -686,21 +698,21 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>45271.347222511577</v>
-      </c>
-      <c r="B8" s="14">
-        <v>1</v>
-      </c>
-      <c r="C8" s="14">
+        <v>45271.354167013887</v>
+      </c>
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11">
         <v>80</v>
       </c>
-      <c r="D8" s="14">
-        <v>2</v>
-      </c>
-      <c r="E8" s="14">
+      <c r="D8" s="11">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11">
         <v>29</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="11">
         <v>2</v>
       </c>
       <c r="G8" s="3">
@@ -711,21 +723,21 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>45271.354167013887</v>
-      </c>
-      <c r="B9" s="14">
-        <v>0</v>
-      </c>
-      <c r="C9" s="14">
+        <v>45271.361111516206</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11">
         <v>88</v>
       </c>
-      <c r="D9" s="14">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14">
+      <c r="D9" s="11">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11">
         <v>20</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="11">
         <v>1</v>
       </c>
       <c r="G9" s="3">
@@ -736,21 +748,21 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>45271.361111516206</v>
-      </c>
-      <c r="B10" s="14">
-        <v>1</v>
-      </c>
-      <c r="C10" s="14">
+        <v>45271.368056018517</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11">
         <v>67</v>
       </c>
-      <c r="D10" s="14">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14">
+      <c r="D10" s="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11">
         <v>33</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="11">
         <v>1</v>
       </c>
       <c r="G10" s="3">
@@ -760,22 +772,22 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>45271.368056018517</v>
-      </c>
-      <c r="B11" s="14">
-        <v>0</v>
-      </c>
-      <c r="C11" s="14">
+      <c r="A11" s="14">
+        <v>45271.375000520835</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11">
         <v>63</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="11">
         <v>3</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="11">
         <v>21</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="11">
         <v>1</v>
       </c>
       <c r="G11" s="3">
@@ -785,22 +797,22 @@
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>45271.375000520835</v>
-      </c>
-      <c r="B12" s="15">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15">
+      <c r="A12" s="15">
+        <v>45271.381945023146</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="12">
         <v>83</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>3</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <v>22</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="12">
         <v>2</v>
       </c>
       <c r="G12" s="3">
@@ -810,8 +822,8 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>45377.659722222219</v>
+      <c r="A13" s="16">
+        <v>45377.666666666664</v>
       </c>
       <c r="B13" s="3">
         <v>3</v>
@@ -828,7 +840,7 @@
       <c r="F13" s="3">
         <v>0</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="9">
         <v>14</v>
       </c>
       <c r="H13" s="2"/>
@@ -837,7 +849,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>45377.666666666664</v>
+        <v>45377.673611053244</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
@@ -854,13 +866,13 @@
       <c r="F14" s="3">
         <v>2</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>45377.673611053244</v>
+        <v>45377.680555497682</v>
       </c>
       <c r="B15" s="3">
         <v>2</v>
@@ -877,13 +889,13 @@
       <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="8">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>45377.680555497682</v>
+        <v>45377.687499942127</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -900,13 +912,13 @@
       <c r="F16" s="3">
         <v>1</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="7">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>45377.687499942127</v>
+        <v>45377.694444386572</v>
       </c>
       <c r="B17" s="3">
         <v>2</v>
@@ -923,13 +935,13 @@
       <c r="F17" s="3">
         <v>1</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="8">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>45377.694444386572</v>
+      <c r="A18" s="14">
+        <v>45377.701388831018</v>
       </c>
       <c r="B18" s="3">
         <v>3</v>
@@ -946,13 +958,13 @@
       <c r="F18" s="3">
         <v>2</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="7">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>45377.701388831018</v>
+      <c r="A19" s="15">
+        <v>45377.708333275463</v>
       </c>
       <c r="B19" s="3">
         <v>2</v>
@@ -969,27 +981,27 @@
       <c r="F19" s="3">
         <v>3</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="13">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>45391.333333333336</v>
-      </c>
-      <c r="B20" s="7">
+      <c r="A20" s="6">
+        <v>45391.340277777781</v>
+      </c>
+      <c r="B20" s="5">
         <v>3</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="5">
         <v>78</v>
       </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
         <v>41</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="5">
         <v>0</v>
       </c>
       <c r="G20" s="3">
@@ -997,8 +1009,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>45391.340277777781</v>
+      <c r="A21" s="6">
+        <v>45391.347222222219</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -1020,8 +1032,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
-        <v>45391.347222222219</v>
+      <c r="A22" s="6">
+        <v>45391.354166666664</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
@@ -1043,8 +1055,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
-        <v>45391.354166666664</v>
+      <c r="A23" s="6">
+        <v>45391.361111111109</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
@@ -1066,8 +1078,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
-        <v>45391.361111111109</v>
+      <c r="A24" s="6">
+        <v>45391.368055555555</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
@@ -1089,8 +1101,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
-        <v>45391.368055555555</v>
+      <c r="A25" s="17">
+        <v>45391.37499971065</v>
       </c>
       <c r="B25" s="3">
         <v>4</v>
@@ -1107,27 +1119,27 @@
       <c r="F25" s="3">
         <v>3</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="10">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
-        <v>45391.666666666664</v>
-      </c>
-      <c r="B26" s="7">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7">
+      <c r="A26" s="6">
+        <v>45391.673611111109</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5">
         <v>103</v>
       </c>
-      <c r="D26" s="7">
-        <v>2</v>
-      </c>
-      <c r="E26" s="7">
+      <c r="D26" s="5">
+        <v>2</v>
+      </c>
+      <c r="E26" s="5">
         <v>21</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="5">
         <v>1</v>
       </c>
       <c r="G26" s="3">
@@ -1135,8 +1147,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
-        <v>45391.673611111109</v>
+      <c r="A27" s="6">
+        <v>45391.680555497682</v>
       </c>
       <c r="B27" s="3">
         <v>2</v>
@@ -1158,8 +1170,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
-        <v>45391.680555497682</v>
+      <c r="A28" s="6">
+        <v>45391.687499942127</v>
       </c>
       <c r="B28" s="3">
         <v>2</v>
@@ -1181,8 +1193,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
-        <v>45391.687499942127</v>
+      <c r="A29" s="6">
+        <v>45391.694444386572</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
@@ -1204,8 +1216,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
-        <v>45391.694444386572</v>
+      <c r="A30" s="6">
+        <v>45391.701388831018</v>
       </c>
       <c r="B30" s="3">
         <v>1</v>
@@ -1227,8 +1239,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
-        <v>45391.701388831018</v>
+      <c r="A31" s="17">
+        <v>45391.708332986113</v>
       </c>
       <c r="B31" s="3">
         <v>4</v>
@@ -1245,27 +1257,27 @@
       <c r="F31" s="3">
         <v>3</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="10">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
-        <v>45391.833333333336</v>
-      </c>
-      <c r="B32" s="7">
-        <v>1</v>
-      </c>
-      <c r="C32" s="7">
+      <c r="A32" s="6">
+        <v>45391.840277777781</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5">
         <v>69</v>
       </c>
-      <c r="D32" s="7">
-        <v>0</v>
-      </c>
-      <c r="E32" s="7">
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
         <v>14</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="5">
         <v>2</v>
       </c>
       <c r="G32" s="3">
@@ -1273,8 +1285,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
-        <v>45391.840277777781</v>
+      <c r="A33" s="6">
+        <v>45391.847222222219</v>
       </c>
       <c r="B33" s="3">
         <v>0</v>
@@ -1296,8 +1308,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
-        <v>45391.847222222219</v>
+      <c r="A34" s="6">
+        <v>45391.854166666664</v>
       </c>
       <c r="B34" s="3">
         <v>1</v>
@@ -1319,8 +1331,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
-        <v>45391.854166666664</v>
+      <c r="A35" s="6">
+        <v>45391.861111111109</v>
       </c>
       <c r="B35" s="3">
         <v>0</v>
@@ -1342,8 +1354,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
-        <v>45391.861111111109</v>
+      <c r="A36" s="6">
+        <v>45391.868055555555</v>
       </c>
       <c r="B36" s="3">
         <v>1</v>
@@ -1365,8 +1377,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
-        <v>45391.868055555555</v>
+      <c r="A37" s="6">
+        <v>45391.87499971065</v>
       </c>
       <c r="B37" s="3">
         <v>0</v>

</xml_diff>